<commit_message>
Code studies oct 2020
</commit_message>
<xml_diff>
--- a/Python/PlayPython/Logbook summary/sum.xlsx
+++ b/Python/PlayPython/Logbook summary/sum.xlsx
@@ -14,11 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>INSTRUMENTS ACTUAL</t>
+  </si>
+  <si>
+    <t>INSTRUMENTS FSTD</t>
+  </si>
+  <si>
+    <t>FSTD</t>
+  </si>
   <si>
     <t xml:space="preserve">SINGLE DAY DUAL </t>
   </si>
   <si>
+    <t>SINGLE DAY PIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE NIGHT DUAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE NIGHT PIC </t>
+  </si>
+  <si>
     <t>DATE LAST FLOWN</t>
   </si>
   <si>
@@ -26,6 +44,33 @@
   </si>
   <si>
     <t>C 150</t>
+  </si>
+  <si>
+    <t>C 172</t>
+  </si>
+  <si>
+    <t>C 210</t>
+  </si>
+  <si>
+    <t>C 210 T</t>
+  </si>
+  <si>
+    <t>FRASCA</t>
+  </si>
+  <si>
+    <t>P 28 A 140</t>
+  </si>
+  <si>
+    <t>P 28 A 180</t>
+  </si>
+  <si>
+    <t>P28 A 160</t>
+  </si>
+  <si>
+    <t>PA 28 R 180</t>
+  </si>
+  <si>
+    <t>X 297</t>
   </si>
 </sst>
 </file>
@@ -387,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -403,16 +448,313 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>6.5</v>
+      </c>
+      <c r="F2">
+        <v>0.6</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>44035</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>5.9</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>6.8</v>
+      </c>
+      <c r="F3">
+        <v>25.2</v>
+      </c>
+      <c r="G3">
+        <v>12.2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>43540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>42040</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>43053</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>41839</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2.6</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>43274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1.6</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>42782</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>51.3</v>
+      </c>
+      <c r="F9">
+        <v>15.9</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>41842</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>41977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>6.399999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>43246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>